<commit_message>
Reviewed all problemematic hospitals 3 groups. 1 Those that are blocked or closed 2 Those that have missing people This is a parsing issue and hopefully sovled when we begin to move to a single source of truth for names and titles 3 those that require manual entry some for blocked sites some for javascript and some with difficutl html that are messed up Next iteration will be to create a baseline dataframe. and then move to singleprocess for names and title verification.
</commit_message>
<xml_diff>
--- a/tracking/FUTURE_WORK_TRACKING.xlsx
+++ b/tracking/FUTURE_WORK_TRACKING.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="29231"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="29328"/>
   <workbookPr defaultThemeVersion="202300"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\ExecutiveSearchYaml\tracking\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9307C362-76BA-4ED0-8AB8-6205FE70C6CA}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8397FE7F-3F8E-4AAD-BE66-76DE4BBE0A5C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="5400" yWindow="1840" windowWidth="16690" windowHeight="17860" activeTab="2" xr2:uid="{B3191408-E674-4EE2-9D0E-8CE05EC6EC45}"/>
+    <workbookView xWindow="15780" yWindow="2500" windowWidth="16690" windowHeight="17860" activeTab="2" xr2:uid="{B3191408-E674-4EE2-9D0E-8CE05EC6EC45}"/>
   </bookViews>
   <sheets>
     <sheet name="Category Summary" sheetId="1" r:id="rId1"/>
@@ -38,7 +38,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="116" uniqueCount="81">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="117" uniqueCount="82">
   <si>
     <t>Category</t>
   </si>
@@ -281,6 +281,9 @@
   </si>
   <si>
     <t>https://www.headwatershealth.ca/who-we-are/governance/executive-leadership-team/</t>
+  </si>
+  <si>
+    <t>627 and 650  have the titles enclosed in "() " Lets note the "()" issue and if it comes up again we can think about a pattern</t>
   </si>
 </sst>
 </file>
@@ -1050,10 +1053,10 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{A1FADFA7-0183-491A-B377-BE9BEEC21271}">
-  <dimension ref="A1:H11"/>
+  <dimension ref="A1:H13"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C10" sqref="C10"/>
+    <sheetView tabSelected="1" topLeftCell="A7" workbookViewId="0">
+      <selection activeCell="B13" sqref="B13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5"/>
@@ -1299,6 +1302,14 @@
       </c>
       <c r="H11" s="2" t="s">
         <v>62</v>
+      </c>
+    </row>
+    <row r="13" spans="1:8">
+      <c r="A13" s="2">
+        <v>627</v>
+      </c>
+      <c r="B13" t="s">
+        <v>81</v>
       </c>
     </row>
   </sheetData>

</xml_diff>